<commit_message>
updated current json file used in app and started work on spell database.
</commit_message>
<xml_diff>
--- a/Data/SpellBook.xlsx
+++ b/Data/SpellBook.xlsx
@@ -13,11 +13,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Spell Name</t>
   </si>
   <si>
+    <t>Spell Level</t>
+  </si>
+  <si>
     <t>Spell Type</t>
   </si>
   <si>
@@ -37,6 +40,127 @@
   </si>
   <si>
     <t>Higher Level Modification</t>
+  </si>
+  <si>
+    <t>Blade Ward</t>
+  </si>
+  <si>
+    <t>Abjuration cantrip</t>
+  </si>
+  <si>
+    <t>1 action</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>V, S</t>
+  </si>
+  <si>
+    <t>1 round</t>
+  </si>
+  <si>
+    <t>You extend your hand and trace a sigil of warding in the air. Until the end of your next turn, you have resistance against bludgeoning, piercing and slashing damage dealt by weapon attacks.</t>
+  </si>
+  <si>
+    <t>Dancing Lights</t>
+  </si>
+  <si>
+    <t>Evocation cantrip</t>
+  </si>
+  <si>
+    <t>120 feet</t>
+  </si>
+  <si>
+    <t>V, S, M</t>
+  </si>
+  <si>
+    <t>Concentration, up to 1 minute</t>
+  </si>
+  <si>
+    <t>You create up to four torch-sized lights within range, making them appear as torches, lanterns or glowing orbs that hover in the air for the duration. You can also combine the four lights into one glowing vaguely humanoid form of medium size. Whichever form you choose, each light sheds dim light in a 10-foot radius. As a bonus action on your turn you can move the lights up to 60-feet to a new spot within range. A light mist be within 20 feet of another light created by this spell and the light winks out if it exceeds the spell’s range.</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
+    <t>Enchantment cantrip</t>
+  </si>
+  <si>
+    <t>S, M</t>
+  </si>
+  <si>
+    <t>For the duration you have advantage on all Charisma checks directed at one creature of your choice that isn’t hostile to you. When the spell ends the creature realises that you used magic to influence it’s mood and becomes hostile to you. A creature prone to violence might attack you. Another creature might seek retribution in other ways (at the DMs discretion) depending on the nature of your interaction with it.</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Touch</t>
+  </si>
+  <si>
+    <t>V, M</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
+  </si>
+  <si>
+    <t>You touch one object that is no larger than 10 feet in any dimension. Until the spell ends, the object sheds bight light in a 20 foot radius and dim light for an additional 20 feet. The light can be coloured as you like. Completely covering the object with something opaque blocks the light. The spell ends if you cast it again or dismiss it as an action. If you target an object held or worn by a hostile creature, that creature must succeed on a Dexterity saving throw to avoid the spell.</t>
+  </si>
+  <si>
+    <t>Mage Hand</t>
+  </si>
+  <si>
+    <t>Conjuration cantrip</t>
+  </si>
+  <si>
+    <t>30 feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V, S, M </t>
+  </si>
+  <si>
+    <t>8 Hours</t>
+  </si>
+  <si>
+    <t>A spectral, floating hand appears at a point you choose within range. The hand lasts for the duration or until you dismiss it as an action. The hand vanishes if it is ever more than 30 feet away from you or if you cast this spell again. You can use your action to control the hand to manipulate an object, open and unlocked door or container, stow or retrieve an item from an open container, or pour the contents out of a vial. You can move the hand up to 30 feet each time you use it. The hand can’t attack, activate magic items or carry more than 10 pounds.</t>
+  </si>
+  <si>
+    <t>Mending</t>
+  </si>
+  <si>
+    <t>Transmutation cantrp</t>
+  </si>
+  <si>
+    <t>1 Minute</t>
+  </si>
+  <si>
+    <t>Instantaneous</t>
+  </si>
+  <si>
+    <t>This spell repairs a single break or tear in an object you touch, such as a broken chain link, two halves of a broken key, a torn cloak, or a leaking wineskin. As long as the break is no larger than 1 foot in any dimension you mend it, leaving no trace of the former damage. This spell can physically repair a magic item or construct but the spell can’t restore magic to such an object.</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You point your finger toward a creature within range and whisper a message. The target (and only the target) hears the message and can reply in a whisper that only you can hear. You can cast this spell through solid objects if you are familiar with the target and know it is beyond the barrier. Magical silence, 1 foot of stone, 1 inch of common metal, a thin sheet of lead or 3 feet of wood blocks the spell. The spell doesn't have to follow a straight line and can travel freely around corners or through openings.
+</t>
+  </si>
+  <si>
+    <t>"desc": "You point your finger toward a creature within range and whisper a message. The target (and only the target) hears the message and can reply in a whisper that only you can hear. You can cast this spell through solid objects if you are familiar with the target and know it is beyond the barrier. Magical silence, 1 foot of stone, 1 inch of common metal, a thin sheet of lead or 3 feet of wood blocks the spell. The spell doesn't have to follow a straight line and can travel freely around corners or through openings.",</t>
+  </si>
+  <si>
+    <t>Minor Illusion</t>
+  </si>
+  <si>
+    <t>Prestidigitation</t>
+  </si>
+  <si>
+    <t>True Strike</t>
+  </si>
+  <si>
+    <t>Vicious Mockery</t>
   </si>
 </sst>
 </file>
@@ -46,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -58,12 +182,22 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -89,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -112,32 +246,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -159,6 +373,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1390,23 +1605,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozenSplit"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.7422" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7422" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7422" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7422" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7422" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7422" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7422" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7422" style="1" customWidth="1"/>
-    <col min="9" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.9141" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="71.1562" style="1" customWidth="1"/>
+    <col min="9" max="9" width="89.4219" style="1" customWidth="1"/>
+    <col min="10" max="10" width="89.4219" style="1" customWidth="1"/>
+    <col min="11" max="11" width="89.4219" style="1" customWidth="1"/>
+    <col min="12" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.55" customHeight="1">
@@ -1434,216 +1650,284 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" ht="65" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" ht="53" customHeight="1">
+      <c r="A4" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s" s="6">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" ht="53" customHeight="1">
+      <c r="A5" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" ht="65" customHeight="1">
+      <c r="A6" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s" s="6">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s" s="6">
+        <v>36</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" ht="41" customHeight="1">
+      <c r="A7" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s" s="6">
+        <v>41</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" ht="77" customHeight="1">
+      <c r="A8" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s" s="6">
+        <v>43</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" t="s" s="6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" t="s" s="4">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" t="s" s="4">
+        <v>47</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1659,65 +1943,76 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:I23"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="0.25" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.25" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="6" customWidth="1"/>
-    <col min="9" max="9" width="12.25" style="6" customWidth="1"/>
-    <col min="10" max="256" width="12.25" style="6" customWidth="1"/>
+    <col min="1" max="1" width="1" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.25" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.25" style="7" customWidth="1"/>
+    <col min="10" max="256" width="12.25" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="2" customHeight="1"/>
+    <row r="1" ht="8" customHeight="1">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="10"/>
+    </row>
     <row r="2" ht="32.55" customHeight="1">
+      <c r="A2" s="11"/>
       <c r="B2" t="s" s="2">
         <v>0</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="20.55" customHeight="1">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="B4" s="3"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1727,8 +2022,9 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1737,7 +2033,8 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="B6" s="3"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1747,7 +2044,8 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="B7" s="3"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1757,7 +2055,8 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="B8" s="3"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1767,7 +2066,8 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="B9" s="3"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1777,7 +2077,8 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="B10" s="3"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1787,7 +2088,8 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="B11" s="3"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1797,7 +2099,8 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
-      <c r="B12" s="3"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1805,116 +2108,6 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="B13" s="3"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="B14" s="3"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="B15" s="3"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="B18" s="3"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="B19" s="3"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="B21" s="3"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="B22" s="3"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="B23" s="3"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>